<commit_message>
added vscode directory to gitignore
</commit_message>
<xml_diff>
--- a/log/Twitter.xlsx
+++ b/log/Twitter.xlsx
@@ -320,345 +320,379 @@
     <t>100</t>
   </si>
   <si>
-    <t>RT @UnCefran: ce genre de shlag https://t.co/AQ5OQhwndX</t>
-  </si>
-  <si>
-    <t>RT @tonycrust: Bulk and Skull were TRAILBLAZERS of Punk fashion. #powerrangers #twitch #marathon https://t.co/85isT9EhOq</t>
-  </si>
-  <si>
-    <t>RT @leomiklasz: Joanna, Polish in Scotland -"I feel like a patient on the operating table...and Scotland is holding my hand saying everythi…</t>
-  </si>
-  <si>
-    <t>RT @SiouxweetNSauer: I didn't even know Sesame Street was on the Twitters...my day is now made. *inner child screams with joy* https://t.co…</t>
-  </si>
-  <si>
-    <t>RT @DougKyed: Fun fact: Joe Thuney has a lower BMI than Eddie Lacy right now. https://t.co/Sutwaj1GAb</t>
-  </si>
-  <si>
-    <t>RT @tribunbesiktas: Türkiye Futbol Direktörü (!) Fatih Terim: "Umarım bu sezon UEFA Avrupa Ligi'ni Roma kazanır." https://t.co/70yg0HpPPQ</t>
-  </si>
-  <si>
-    <t>RT @latefah_s11: أتأمل مكّة! أتأمّل كيف لدعوة أن تحوّل هذا المكان الأجدب القاسي لوطنٍ تتمنّى القلوب جواره ؟ 
-بالدعاء يخضرّ خريفك ، قل : يـ…</t>
-  </si>
-  <si>
-    <t>RT @sh888er: .
-غداً الأربعاء ٦/١٥
-ضيفنا الشيخ : محمد العامر 
-لقاء بعنوان : ( أهمية الوقت ) ??
-في #شبابنا_غير
-.
-حياكم الله جميعاً ???? https://…</t>
-  </si>
-  <si>
-    <t>#MariasParaMelos #NiUnaMenos #MelosParaYa #Opresor #Machirulo 
-@Melosdead ???? https://t.co/yJM3EnaCnU</t>
-  </si>
-  <si>
-    <t>RT @SEV_gob_mx: Personal de #SEV se capacita en primeros auxilios. https://t.co/1lrLk9aDYW @YoconYunes @Enrique_PerezR @GobiernoVer #Veracr…</t>
-  </si>
-  <si>
-    <t>RT @afrispheric: EFCC is now running motivational workshops...
-Lol... https://t.co/Dz9qJ1tT5G</t>
-  </si>
-  <si>
-    <t>https://t.co/SuAtgsSoiQ</t>
-  </si>
-  <si>
-    <t>@SanJoseSharks @RyanNolan79 @Bakes_Jamie13 @sharkvoice @DanRusanowsky @GregCappellaro @doc_doyle @BelfastGiants… https://t.co/cxxgpWTP6Z</t>
-  </si>
-  <si>
-    <t>RT @peterdaou: All of this mess, every last bit of it, is because the media, left and right wantonly smeared and slandered this lifelong pu…</t>
-  </si>
-  <si>
-    <t>RT @jonyrahal: Esta es la razón por la cual el pueblo de Tacarigua del Municipio GÓMEZ no le llega el agua. #ElCentralismoEsCorrupción @hid…</t>
-  </si>
-  <si>
-    <t>RT @totorangelm: #HonorableTraidor Guillermo Antonio Santos del @PartidoLiberal no olvidar https://t.co/SgBygO7s2x</t>
-  </si>
-  <si>
-    <t>https://t.co/h0KFmr27kX</t>
-  </si>
-  <si>
-    <t>RT @MailOnline: See where the toppling of the tsars all started in dazzling St Petersburg, Russia https://t.co/1PYOrRdGpC https://t.co/gjms…</t>
-  </si>
-  <si>
-    <t>They only give them allowances here on Twitter.</t>
-  </si>
-  <si>
-    <t>Internet lo sabe todo: https://t.co/C6iQBttlZ2</t>
-  </si>
-  <si>
-    <t>RT @doktordin: Al sepetten bir zerzevat daha: ''Namaz kılmayanları öldürün.''
-(Peki Yolsuzluk ve Rüşvet Yiyenleri Ne Yapıyoruz) https://t.…</t>
-  </si>
-  <si>
-    <t>RT @RT_russian: В Крым прибыла делегация сербских политиков https://t.co/GjDkLqjAvk https://t.co/NAFxW6krtr</t>
-  </si>
-  <si>
-    <t>RT @KramponluPisago: Kayserispor'dan Barcelona'ya deneme antrenmanlarına giden 13 yaşındaki Emre Demir için 'Üstün futbol zekasına sahip' r…</t>
-  </si>
-  <si>
-    <t>RT @airlinem: The Legend of Zelda: Breath of the Wild is a masterpiece (and the highest grade I've ever given) https://t.co/cXwVe0YirJ via…</t>
-  </si>
-  <si>
-    <t>RT @3bdualr7man: مع تسارع الحياة وفي ظل عالم امتلأ تعقيدا يكون الحنين لحياة البساطة التي عشناها سابقا كثيرا ما نشتاق لها
-#عمان_المجد https:…</t>
-  </si>
-  <si>
-    <t>RT @CCONFISSOES: uouuu https://t.co/ChU4tYyXS4</t>
-  </si>
-  <si>
-    <t>RT @TowsAndHoes: https://t.co/3bilcxekwd</t>
-  </si>
-  <si>
-    <t>RT @q8_nabd: طفل مفقود موجود في مخفر سلوى https://t.co/XfDTgGwD5P</t>
-  </si>
-  <si>
-    <t>RT @cloveochai: i've been gay for a fish since before i knew i was gay, this ain't news. https://t.co/Jov3NhFKG8</t>
-  </si>
-  <si>
-    <t>@B8CSP0RF @VineCreators https://t.co/HmpSSIh26a</t>
-  </si>
-  <si>
-    <t>RT @PigzyNatt: พ่ายแพ้ให้กับแม่เลี้ยงในลุคนี้มากค่ะ หลวยที่แท้จริงค่ะคุณขาาาา #บ่วงหงส์ https://t.co/e05zP8u7TG</t>
-  </si>
-  <si>
-    <t>RT @zaralrba: @hmy__h ❤
-#المتألقه_10K_Meem_متابع
-مبرووووك شاهدين لك بالخير 
-#انيقه 
-#مبدعه 
-#رائعه #بحضورها
-????????????????????
-#حساب_جميل https://t…</t>
-  </si>
-  <si>
-    <t>"Antes se daban una vuelta de 30 km para llegar a Tendales y Bajo Alto hoy lo hacen en 8km lineales" https://t.co/LyK2w0JiET</t>
-  </si>
-  <si>
-    <t>RT @ajplus: Canadian cystic fibrosis patients live 10 yrs longer than U.S. counterparts. Researchers credit diet, insurance, &amp;amp; access to tr…</t>
-  </si>
-  <si>
-    <t>영상전보벌레를 붙잡았습니다!
-놀랍게도…Mr.0의 얼굴 촬영에 성공했습니다 !!!
-https://t.co/t8hXqHArOQ #트레크루 https://t.co/wTHHPTCrYK</t>
-  </si>
-  <si>
-    <t>영상전보벌레 발견!
-아론 일당을 순간 포착했습니다!
-https://t.co/jPZcHvevl2 #트레크루 https://t.co/60zrIdnSsT</t>
-  </si>
-  <si>
-    <t>RT @Nnedi: As a black woman writing a black female main character in a scifi novel, seeing my character whitewashed on the cover felt-like-…</t>
-  </si>
-  <si>
-    <t>RT @NewFriki: Cuando te ves el último capítulo de un anime... pero al final del capítulo sale que habrá otra temporada.... https://t.co/355…</t>
-  </si>
-  <si>
-    <t>RT @Clothiies: https://t.co/LWF0RRuUdZ</t>
-  </si>
-  <si>
-    <t>RT @cakeke29: Jaehee x Mc
-#mysticmessenger https://t.co/O1me3G6Y2k</t>
-  </si>
-  <si>
-    <t>RT @XHNews: Cherry blossoms are covered with ice after blizzard hits Washington DC #blizzard2017 #stella https://t.co/p062EQLuUX</t>
-  </si>
-  <si>
-    <t>RT @allidoislovemc: That moment you realize that @MariahCarey is always gonna be a skinnier legend than you &amp;amp; u can't do a thing about it.…</t>
-  </si>
-  <si>
-    <t>RT @SENIAT_Oficial: ???? Las Personas Naturales pueden realizar el proceso de declaración del #ISLR de manera rápida a través del Portal http…</t>
-  </si>
-  <si>
-    <t>Pero qué he hecho https://t.co/YKv3RKTpfU</t>
-  </si>
-  <si>
-    <t>RT @SergioRamos: Pon un Sergio en tu vida ?? 
-Put a little Sergio in your life ??
-@23Llull https://t.co/lAusyai6xd</t>
-  </si>
-  <si>
-    <t>@mehdii_94 https://t.co/uvEEpC4LRg</t>
-  </si>
-  <si>
-    <t>RT @AdelAliBinAli: اللهم 
-إني اسألك حبك 
-وحب من يحبك 
-وحب كل عمل 
-يقربنا إلى حبك https://t.co/R85EmqB8Q2</t>
-  </si>
-  <si>
-    <t>RT @badestoutfits: https://t.co/DQFZuuorC5</t>
-  </si>
-  <si>
-    <t>RT @tamamoebot: [Moe bot][#3598] Christina maid [#steinsGate] https://t.co/5npSZUWyUl</t>
-  </si>
-  <si>
-    <t>RT @akinosora0726: マリー https://t.co/xd4oEl7E4L</t>
-  </si>
-  <si>
-    <t>RT @vffarias99: Vem ai LETS GO PRIVILEGE, um novo conceito de evento. Um publico selecionado a dedo em um local maravilhoso com uma vibe ún…</t>
-  </si>
-  <si>
-    <t>RT @v_xv_xv: جِئت نحوي مطراً كيف أخفي الغيث عني ، 
-كيف أنفي زهرة صارت بأضلاعي تُغني ® https://t.co/srLMyS0UWs</t>
-  </si>
-  <si>
-    <t>OBRAS MAESTRAS DE BUDAPEST | Museo Thyssen | 24 marzo, 10:15 h. Contacto: 915231781 cibeles@cibelescultura.org https://t.co/Kae38iUxAz</t>
-  </si>
-  <si>
-    <t>?????? https://t.co/lhTnK2lNMC</t>
-  </si>
-  <si>
-    <t>RT @ruben_aybar: #ProgramaLideresVisitantes y #LideresRDenUSA ahora en CNN WASHINGTON. @ElicFernandez https://t.co/KFhYSpqExe https://t.co/…</t>
-  </si>
-  <si>
-    <t>RT @RealKyleMorris: Where is the intolerant left speaking out against how inhumane and threatening this is to America? #doublestandards htt…</t>
-  </si>
-  <si>
-    <t>Bunu biliriz vede müthiş lezzet https://t.co/kcw7A0YiPz</t>
-  </si>
-  <si>
-    <t>RT @officialkhy_ri: Definitely just a video https://t.co/R0YlVHZ8CQ</t>
-  </si>
-  <si>
-    <t>lol i see stuff like this and i'm like why r u so salty??? like i work a full time job n don't go to college. they… https://t.co/Pw3yi5fzVI</t>
-  </si>
-  <si>
-    <t>RT @mm231m: https://t.co/CMJhKuJ4ZF</t>
-  </si>
-  <si>
-    <t>RT @VGFGamers: Ouch ?? https://t.co/oxDyqiq59S</t>
-  </si>
-  <si>
-    <t>RT @kimmingyugyu: 아 나 심장 진짜;;;;;;;;;;; 민규야 예고 좀 하고 가까이 와줄래?;;;;;;;;;;;;:: https://t.co/sw1ffs0n7Y</t>
-  </si>
-  <si>
-    <t>Obviously I need the details on this one https://t.co/WcBCcMu8m7</t>
-  </si>
-  <si>
-    <t>RT @okkcjj: OML https://t.co/BKtX2iFeY6</t>
-  </si>
-  <si>
-    <t>RT @PAYNOFOBICS: ~Vitaly Voronko
-ja to bym mu z marszu dała I miejsce, uwielbiam jego występXDDD https://t.co/2SPlyfszLg</t>
-  </si>
-  <si>
-    <t>https://t.co/49EIecTHMI</t>
-  </si>
-  <si>
-    <t>RT @Alextrxm: quand j'essaye de dormir mais que j'me souviens d'un truc gênant que j'ai fais il y a 2 ans https://t.co/ZVy2qi0v3L</t>
-  </si>
-  <si>
-    <t>さてと、卒業旅行に行く娘らを起こすのだ??このまま寝ずに朝やな??そして今日も仕事頑張る??ホルンから働くエネルギーもらったから大丈夫❗
-ああ、勝つって素晴らしい??
-#SVhorn https://t.co/irXyQU4RKv</t>
-  </si>
-  <si>
-    <t>https://t.co/yfyCzVcLJR</t>
-  </si>
-  <si>
-    <t>RT @pozzanipw: Fancy winning a filtered water bottle? Just Flw&amp;amp;RT for a chance to #win #comp #giveaway #competition #mondaymotivation winne…</t>
-  </si>
-  <si>
-    <t>Который раз играю, а всё равно впечатляет #METRO2033 #PS4share https://t.co/Y0h0rQfKgt</t>
-  </si>
-  <si>
-    <t>RT @chanelpuke: when you switch lanes and the lane you left starts moving faster https://t.co/EgKgmNOaAa</t>
-  </si>
-  <si>
-    <t>RT @splcenter: If you had to appear in court for a traffic ticket/misdemeanor Alexander City's judge didn't ask if you can pay fees https:/…</t>
-  </si>
-  <si>
-    <t>RT @kierraaaw: he was In N Out of my guts after this pic ??❤️?? https://t.co/dm5o3LDny0</t>
-  </si>
-  <si>
-    <t>RT @imshapoppin: him: i need me a lil baby who gone listeeeennnnnnn
-me: https://t.co/uToEBTyGl0</t>
-  </si>
-  <si>
-    <t>RT @niftyvibe: https://t.co/QQE0VemFtf</t>
-  </si>
-  <si>
-    <t>RT @thetestpit: #Win a Nintendo Plushes bundle from @JAKKStoys in our latest #competition. Follow &amp;amp; RT. https://t.co/Ee9CjJflXT #giveaway #…</t>
-  </si>
-  <si>
-    <t>https://t.co/ZynfzbIQUh</t>
-  </si>
-  <si>
-    <t>RT @sofieeriksen3: SHOP HERE: https://t.co/q6c4C09yPa 
-#hvisk #jewellery #fashion #pendant #gold #silver #lace #wild #collarbone #bw #mono…</t>
-  </si>
-  <si>
-    <t>RT @WSHHFANS: When people are fighting in your mentions and forget to untag you https://t.co/7L8dv5QXX0</t>
-  </si>
-  <si>
-    <t>RT @partypartynails: ummmm this made my week https://t.co/B412dXbPcZ</t>
-  </si>
-  <si>
-    <t>RT @Clothiies: https://t.co/Ogf2NwnfEy</t>
-  </si>
-  <si>
-    <t>RT @lexj35: I call when i want 
-I call when i want 
-I call when i want 
-I call when i want https://t.co/nsEJ55yCuy</t>
-  </si>
-  <si>
-    <t>RT @LibyaLiberty: can that skull run for higher office? https://t.co/Or30NfJYpv</t>
-  </si>
-  <si>
-    <t>@richardfarley I do not like twitter spam, said Chard I am.</t>
-  </si>
-  <si>
-    <t>#LeonardSimpsonTV 
-Despite its existence in every show about awkward teenagers, I kind of … https://t.co/7A5vTgVji4 https://t.co/znvzgkhyJm</t>
-  </si>
-  <si>
-    <t>RT @intofilm_edu: Huge thank you to everyone who joined us today at the #IntoFilmAwards! Congratulations to all winners and nominees! https…</t>
-  </si>
-  <si>
-    <t>RT @AnaHG_: https://t.co/cK3synnQnr</t>
-  </si>
-  <si>
-    <t>RT @PurposeTourCom: Look how calm everyone is and no phones are out! How it should be done! https://t.co/5SITyQtJ6Z</t>
-  </si>
-  <si>
-    <t>@mirianmh23 @hennen35 @With_Love_1 @DaaD01 @bobbygreyone @sergey_silkin @val_fina @layebin @YakoutLaila https://t.co/JEcYC5qAwM</t>
-  </si>
-  <si>
-    <t>Shhh Dont tell you wife by @BatMansGF3 - https://t.co/649FCAfvjD @manyvids https://t.co/o4ZxinXlRc</t>
-  </si>
-  <si>
-    <t>#csw61 event on the abolition of the sex trade by @SPACEintl @Embrace_Dignity @CATWIntl Intersection of sex &amp;amp; race,… https://t.co/eOulJc7mck</t>
-  </si>
-  <si>
-    <t>RT @girlgroupspics: ahn sohee https://t.co/f5suoy6v6o</t>
-  </si>
-  <si>
-    <t>RT @Sexy_Lovely_Sam: I'm online right now on @Skyprivate https://t.co/5LawfqVxh6 https://t.co/pyZIXTT0dY</t>
-  </si>
-  <si>
-    <t>RT @Hippy: a very important reminder https://t.co/F4mGP1ku6P</t>
-  </si>
-  <si>
-    <t>RT @Seahawks: We have agreed to terms with RB Eddie Lacy. #GoHawks 
-?? | https://t.co/Ypx0R4i2EG https://t.co/MKvyXSC6Xw</t>
-  </si>
-  <si>
-    <t>RT @aikii: im never going to get to play this game https://t.co/OX5kkIFZ2a</t>
-  </si>
-  <si>
-    <t>RT @tessgrobbenx: "hey can i copy your homework?"
-"yeah just change it a little bit so it won't look too obvious" https://t.co/PbFgewHzjF</t>
-  </si>
-  <si>
-    <t>RT @WORLDSTAR: ?? https://t.co/4fXHo10BIp</t>
-  </si>
-  <si>
-    <t>ㅤ https://t.co/bSdnknbzIF</t>
+    <t>RT @BALKIRAGA: PukKodu ATATÜRK
+Aydınlık izleri silinmedikçe ülke doğruyu bulacaktır.
+@MKAtimi 
+@hzlandrc 
+@B6tur 
+@YildirimUgurgul 
+@zzoguz…</t>
+  </si>
+  <si>
+    <t>RT @tancabrona: — ¿Sigues enojada?
+— No.
+— ¿Y ese cuchillo?
+— https://t.co/oClipdteUA</t>
+  </si>
+  <si>
+    <t>RT @BLACKPINKGLOBAL: [170327] [PRESS] Jennie at BOON THE SHOP Event #BLACKPINK #블랙핑크 #JENNIE #제니 https://t.co/oT8cI2dDFb</t>
+  </si>
+  <si>
+    <t>RT @12Super1Hero: つじ写真館さんに昨日お忙しい時間に行きました！
+びゅうおの写真とコメントをお願いして帰宅しました
+お茶ありがとうございましたm(*_ _)m https://t.co/sDvwhF9zVD</t>
+  </si>
+  <si>
+    <t>RT @The40Chambers: CRICE https://t.co/UySmRmjKo7</t>
+  </si>
+  <si>
+    <t>What a fucking iconic queen. https://t.co/fApuhGZs0b</t>
+  </si>
+  <si>
+    <t>RT @_omanprojects: ??شركة تنمية نفط #عمان تطرح مشروع تطوير رأس الحمراء للاستثمار.. https://t.co/Jid0Plt2zZ</t>
+  </si>
+  <si>
+    <t>RT @gblardone: -2 fois ministre de Fillon (+1,2M chômeurs +600MM dette)
+-2 fois déjà sous Chirac
+-2 fois porte-parole du gouv. dès 1995
+-Dé…</t>
+  </si>
+  <si>
+    <t>RT @debbiemc1547: https://t.co/ZpnA78zNT3</t>
+  </si>
+  <si>
+    <t>RT @AuntyTalks: இந்த மாதிரி ரசிச்சு புண்டைய நக்க யாராவது lesbo Twitter ல இருக்கீங்களா ப்ரண்ட்ஸ்?? https://t.co/lHDcVKw1cB</t>
+  </si>
+  <si>
+    <t>RT @kacsaatolldu: Anasınıfına bile Erdoğan'lı kitap dağıtanlar, Nutuk'u 'siyasi propaganda olur'diye yasaklayalı birkaç gün oldu https://t.…</t>
+  </si>
+  <si>
+    <t>RT @VoetbalInside: PRIMEUR: Hierbij presenteren wij jullie de nieuwe staff van @OnsOranje / @KNVB. Beter? ?? ???? #voetbalinside https://t.co/…</t>
+  </si>
+  <si>
+    <t>https://t.co/FwAYHcSjjx</t>
+  </si>
+  <si>
+    <t>RT @n_nammimi: ผัวเดย์ค่ะ แจกเป๋านี้ 1 ใบ รีไปนะ อิอิ #KINGJACKSONDAY https://t.co/lNsQthhW4m</t>
+  </si>
+  <si>
+    <t>RT @NTelevisa_com: El premio llega en un momento difícil para México porque han sido asesinados 3 periodista en el último mes:@CarlosLoret…</t>
+  </si>
+  <si>
+    <t>RT @Iovekth: this angel https://t.co/gV1dqldcsK</t>
+  </si>
+  <si>
+    <t>Gemüse-Implantate: So sollen aus Spinat Ersatzteile für unser Herz wachsen https://t.co/lTHuSSSsfc https://t.co/DQJhWzysVk</t>
+  </si>
+  <si>
+    <t>RT @tuanarchives: happy birthday to got7's angel, he deserves to be happy and loved, we love him so much, he is always good to mark ✨❤ #KIN…</t>
+  </si>
+  <si>
+    <t>https://t.co/g1OrhO1Fa1</t>
+  </si>
+  <si>
+    <t>They're in Estonia working for Putin. There's NO WAY on EARTH Trump's got 36%, Putinbots are hacking the pollsters… https://t.co/3oZUntzOZA</t>
+  </si>
+  <si>
+    <t>RT @jenarovillamil: "Lo contrario de la libertad no es el determinismo sino el fatalismo": Jean Paul Sartre https://t.co/xRHAvr1FcD</t>
+  </si>
+  <si>
+    <t>RT @deray: what type of society raised this domestic terrorist? https://t.co/XI501hEBVl</t>
+  </si>
+  <si>
+    <t>RT @calzonaflames: "If you love someone, you tell them" #12YearsOfGreysAnatomy *sobs* https://t.co/p7YBmhMBlx</t>
+  </si>
+  <si>
+    <t>RT @Dalton_Chad: Come to the library mall and #VoteColeUmeh !! Dex did, you should too. https://t.co/aiWPHoOzV6</t>
+  </si>
+  <si>
+    <t>RT @RocketJoy: Check out the insides of our Crew Dragon spacecraft and the system that will support human life in space! https://t.co/xUnmE…</t>
+  </si>
+  <si>
+    <t>En el hilo de la semana, pude descargarme está joya. Aprovechen  https://t.co/mmXAYq6QsE https://t.co/lJ0s6I4td1</t>
+  </si>
+  <si>
+    <t>RT @hehehe9988: โอ้ยขรรม?? เจ๊หนิงไลฟ์สดของพี่เป๊กอยู่ แล้วซูมไปที่เป้าเพราะพี่เป๊กบอกพึ่งรู้ตัวว่าเป้าแตก55555555555555 #เป๊กผลิตโชค #ผลิต…</t>
+  </si>
+  <si>
+    <t>これほしい(´･ω･`)
+カラコンも欲しいし。
+今更ながらRuuaのカバンよりこっちにすればよかった、、かも https://t.co/Z6ZrEl8rJD</t>
+  </si>
+  <si>
+    <t>Please present your evidence that causality holds outside of this universe. https://t.co/v0k8R0sPSK</t>
+  </si>
+  <si>
+    <t>【モンスト】『わくりん2倍』で金種大量出現！勝ち組プロスト多数爆誕ｷﾀ━━━━(ﾟ∀ﾟ)━━━━!!【画像あり】⇒ https://t.co/WkI6UNUMrl https://t.co/H1rLHWHezq</t>
+  </si>
+  <si>
+    <t>https://t.co/NRLkmYTh78</t>
+  </si>
+  <si>
+    <t>Skrenggeh! https://t.co/E34n7LOTP1</t>
+  </si>
+  <si>
+    <t>RT @Jukeslol: SALVE RAPEIZE
+ACABAIE DE ACORDAR E STREAM JA ESTA ONLINE
+JOGANDO NA MAIN CHALLENGER
+#enois
+https://t.co/gm1jefJqs8 https://t.…</t>
+  </si>
+  <si>
+    <t>https://t.co/fyFYjKxDqP</t>
+  </si>
+  <si>
+    <t>RT @PaosameSurTwi: Bientôt les gens ils porteront ca oklm dans la rue https://t.co/iQhCA14fnL</t>
+  </si>
+  <si>
+    <t>RT @SeamusGorman1: @Meme_Druid @ReeReeC2 @RandallKraft @Mom2theCorps @ggentlemanirish @Kimmie091577 @JewelsJones1 @jimmygarner @KeecoWang5…</t>
+  </si>
+  <si>
+    <t>RT @atletico: Gostou do clipe #Galo109? Então assista ao making of com os erros de gravação! #Galo #PaixãoDoPovo https://t.co/LzydwyUDF3</t>
+  </si>
+  <si>
+    <t>This man is only accused of 5 billion ruppies of corruption.
+Still a shoe of Zardari 
+ https://t.co/gRDluzDvLq</t>
+  </si>
+  <si>
+    <t>RT @WBCBaseball: Now’s your opportunity to win a sweet prize! RT for a chance to win this! #WBC2017 https://t.co/H9S34RYgrU</t>
+  </si>
+  <si>
+    <t>RT @jvaldez666: Eres flor eres hermosa ?? https://t.co/HB8npfvnFb</t>
+  </si>
+  <si>
+    <t>RT @kirbsterr__: Fr though ?????? I'm fucking tripping https://t.co/8CQXKw4h7G</t>
+  </si>
+  <si>
+    <t>RT @ItsFoodPorn: Blueberry Cheesecake https://t.co/fyhNhlmBts</t>
+  </si>
+  <si>
+    <t>RT @guillaumecastan: Pour lutter contre la concentration des terres par les grandes sociétés agricoles et aider les jeunes agriculteurs, #J…</t>
+  </si>
+  <si>
+    <t>RT @tarrraan_: Come on y'all !! Get me my dream dog ! Please !! https://t.co/nZctc4jIhC</t>
+  </si>
+  <si>
+    <t>nahhh lol https://t.co/AOEzaEJaCU</t>
+  </si>
+  <si>
+    <t>#ابسط_حقوق_المصريين https://t.co/oYx7LpgJUr</t>
+  </si>
+  <si>
+    <t>RT @TolgaYakali: ??31.03.2017 https://t.co/Ln2FQFfU9h</t>
+  </si>
+  <si>
+    <t>RT @baptista1904: QUAL É O MELHOR CLUBE DO MUNDO https://t.co/6HQ4kYMXGx</t>
+  </si>
+  <si>
+    <t>RT @jiminspired: the days where jimin was chubby and buff, the cutest basketball player https://t.co/05yjrLZSXn</t>
+  </si>
+  <si>
+    <t>RT @fyo101: اذا اخوي نام في الصالة
+ وامي قالت وده سريره ?? https://t.co/KCkYzXMfFJ</t>
+  </si>
+  <si>
+    <t>RT @camucha4: URGENTE! Necesitamos Avastin 400 (4 frascos) , para que Melody pueda continuar su tratamiento.  #TodosPorMelody Gracias RT #u…</t>
+  </si>
+  <si>
+    <t>RT @KFCBarstool: God I love Frank Martin https://t.co/euQXXutVg3</t>
+  </si>
+  <si>
+    <t>RT @nia4_trump: On #MuslimWomensDay let's take a moment to understand the etiquette of Wife Beatings according to Islam &amp;amp; Sharia.
+https://t…</t>
+  </si>
+  <si>
+    <t>ENJOY EVERY STEP ALONG THE WAY! https://t.co/ULrzDrwv2D</t>
+  </si>
+  <si>
+    <t>RT @SytnerBMW: Check out this M4 Convertible in Sakhir Orange with Black Individual Merino Leather at Sytner Sheffield. For more info, call…</t>
+  </si>
+  <si>
+    <t>RT @porrachatu: "você deveria ser mais legal" https://t.co/BFD7wsLkm0</t>
+  </si>
+  <si>
+    <t>RT @michaeldweiss: I can't even get my child to put her raincoat on in exchange for Teletubby time. Russia's youth is enterprising. https:/…</t>
+  </si>
+  <si>
+    <t>RT @ArmaTorlk: Pour gagner votre précommande RT + follow me et @armateam :) ! Tirage au sort dimanche 19 à 20h ! #Torlk2017 https://t.co/1X…</t>
+  </si>
+  <si>
+    <t>RT @ehdaora: essa eh pra se apaixona https://t.co/N5MxOFAb03</t>
+  </si>
+  <si>
+    <t>RT @Noelia_Mansilla: Ojala que nunca necesite uno! @Belu_Mansilla https://t.co/beD72KTmoR</t>
+  </si>
+  <si>
+    <t>RT @TeamBangtanCL: Info ??(!!!) 
+¡Big Hit ha respondido ante las amenazas hacia Jimin! 
+#ArmysWillProtectJimin https://t.co/Q1iIAnQ0FF</t>
+  </si>
+  <si>
+    <t>Horario de Noticias CNTP en cntpradio. https://t.co/1M2O36vncn https://t.co/DxtrQwETVI</t>
+  </si>
+  <si>
+    <t>RT @BTS_twt: #노츄
+#커밍순 https://t.co/lRJy5FkevO</t>
+  </si>
+  <si>
+    <t>RT @paulinaromo69: #NewProfilePic https://t.co/nRT2H9l4Z1</t>
+  </si>
+  <si>
+    <t>RT @TheCCCompanies: Living Life Like A G Mixtape Dropping April 28th ??????@Art_Gretzky PROD. BY @DHoodNational @SwaggBBeatz ?????? #indiemusic #…</t>
+  </si>
+  <si>
+    <t>@BlogdenWelttag sagt mal, kann ich das eigentlich auch noch bearbeiten? Also die Twitter- und Facebookzeile zum Beispiel? ??</t>
+  </si>
+  <si>
+    <t>RT @Uber_Pix: Welcome little turtle https://t.co/Q32PdGDUul</t>
+  </si>
+  <si>
+    <t>RT @abcfree56: #歳納京子生誕祭2017 
+#歳納京子
+#ゆるゆり
+#RTした人全員フォローする 
+#いいねした人全員フォロー 
+京子おめでとう????
+トメィトゥトメィトゥ?? https://t.co/lR1hdvJL3c</t>
+  </si>
+  <si>
+    <t>RT @AmanatUllah23: भारत है, तो हम हैं। भारत की प्रगति में ही हर भारतीय की उन्नति है https://t.co/2Te5LSPsCV</t>
+  </si>
+  <si>
+    <t>This is my favourite Mariah song idk why she never liked this song tbh https://t.co/g3HOSLQyqB</t>
+  </si>
+  <si>
+    <t>RT @skinhub: ⭐️ Butterfly Knife | Ultraviolet Giveaway
+* RT &amp;amp; Follow
+* Reply w/ Skinhub User ID
+Winner in 24 Hours! https://t.co/lYNnEezz…</t>
+  </si>
+  <si>
+    <t>RT @LicCarlosSosa: Con ayuda de Dip. Fermín Trujillo, se apoyo al niño Angel Miguel Buitimea Pérez, talento Sonorense.
+#NuevaAlianzaimpulsa…</t>
+  </si>
+  <si>
+    <t>RT @itsyourgamerguy: Had some incredible support for this photo over on Instagram! Great addition to #ForzaHorizon3 @ForzaMotorsport @Xbox…</t>
+  </si>
+  <si>
+    <t>RT @hhuyrrtty04: #사설토토사이트추천
+#사다리사이트추천
+메-이-저-놀-이-터
+♏안전최고♏
+♐♐♐♐♐
+❄https://t.co/jDR4J3anrs❄☜바로가기
+Ⓜ매일e벤~Ⓜ
+♌♌♌♌♌
+☃편안히즐기세요☃
+☑hello☑ https:…</t>
+  </si>
+  <si>
+    <t>RT @DeOlhoBBBrasil: Amoreees!
+Vamos lutar pelo trio #MallyMar e contra:
+Falso moralismo
+Arrogância
+Ganância
+Inveja
+Calunia
+Difamação
+#ForaD…</t>
+  </si>
+  <si>
+    <t>RT @FAVELADOANTARES: Favelado também é gente!
+NÃO DEIXEM ESSE VIDEO MORRER! https://t.co/7QNiUWDS6n</t>
+  </si>
+  <si>
+    <t>Omg @JackMorlenMusic voice is just???? https://t.co/mNvlffw5Qu</t>
+  </si>
+  <si>
+    <t>RT @awecoupIes: this is the perfect representation of me in haunted houses https://t.co/0C1E7PFzAD</t>
+  </si>
+  <si>
+    <t>RT @DucaVisko: Dobro, ima li vođa bar dva validna potpisa od onih 650? Jedan demant za drugim... https://t.co/b3lJQbOWFc</t>
+  </si>
+  <si>
+    <t>Share your thoughts: https://t.co/pkub4F5nO3 https://t.co/0FNc6D1ios</t>
+  </si>
+  <si>
+    <t>Cuando Mami y Papi descubren un feature nuevo en el celular ?? https://t.co/3sXNqwOLig</t>
+  </si>
+  <si>
+    <t>RT @badman_sean: how's it goinggggggg https://t.co/WseFXKlTil</t>
+  </si>
+  <si>
+    <t>Héctor Suárez va a parar al hospital tras sufrir una fuerte caída https://t.co/9kRoKRPQ2D</t>
+  </si>
+  <si>
+    <t>@narendramodi https://t.co/569xmO4gcB</t>
+  </si>
+  <si>
+    <t>RT @ErkanPusmaz: https://t.co/zrnUjqnSLu</t>
+  </si>
+  <si>
+    <t>#GirlPower #WomenLead https://t.co/nGD76ESDlp</t>
+  </si>
+  <si>
+    <t>RT @OulivierJirou: Lavezzi cet arnaqueur ?? https://t.co/MtmajyqkaE</t>
+  </si>
+  <si>
+    <t>RT @FirstTake: "LeBron has done so much for the game... He's earned the opportunity to take a rest." - @kobebryant https://t.co/frQkcalV3N</t>
+  </si>
+  <si>
+    <t>RT @amam_990: @ajmi604 
+•??
+??
+??
+#الامير_العجمى_100k_محب
+شاهدين لـكـ بـالخير يارب
+•??
+??
+??
+#حساب_أفتخر_فيه
+#حساب_ملكي
+????????????
+@ajmi604 
+•??
+??
+#تو…</t>
+  </si>
+  <si>
+    <t>RT @mjulio777pr: I know y'all remember this one. Wisin's verse was ?? https://t.co/7H4UQE8eU6</t>
+  </si>
+  <si>
+    <t>RT @justjamiie: https://t.co/0shbb8bNJe</t>
+  </si>
+  <si>
+    <t>RT @hanxine: Slytherin don't deserve this https://t.co/VO3MBW2v3v</t>
+  </si>
+  <si>
+    <t>RT @3zuwan: Lamborghini Huracan VS 14' CBR 1000RR. Rilek je Lamborghini ni kena tapau. https://t.co/SstzsHdpzN</t>
+  </si>
+  <si>
+    <t>RT @waterparks: HI MOM. WE GOT OUR FIRST MAGAZINE COVER. THIS IS THE COOLEST THING IN THE WORLD. DAMN. https://t.co/tTBFAZuUUj https://t.co…</t>
+  </si>
+  <si>
+    <t>RT @JaMir_Russell: Pure evil lol https://t.co/Is3BIz7rMw</t>
+  </si>
+  <si>
+    <t>RT @caacosta1962: Uds. saben porqué @Lenin no quiso debatir?
+No?
+Yo si se
+Porque no lo dejaron contar cachos de $10,000 https://t.co/rsx…</t>
+  </si>
+  <si>
+    <t>RT @BarstoolUA: Monday morning blues? This should help.
+https://t.co/LvkcCJgBKF</t>
+  </si>
+  <si>
+    <t>RT @heyifeellike: when you're dead inside but you still wanna have a good time. https://t.co/cetDuxQlSi</t>
+  </si>
+  <si>
+    <t>RT @MacCocktail: "When I sing, trouble can sit right on my shoulder and I don't even notice." 
+― Sarah Vaughan (born this day, March 27, 19…</t>
+  </si>
+  <si>
+    <t>RT @Stalinonyou: "Get in loser, we're going shooting" https://t.co/DZVF5NGTVX</t>
   </si>
 </sst>
 </file>

</xml_diff>